<commit_message>
change in Concrete xls file
</commit_message>
<xml_diff>
--- a/BridgesLCA/data/Concrete.xlsx
+++ b/BridgesLCA/data/Concrete.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julien.cravero\source\repos\BridgesLCA\BridgesLCA\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C479116B-7756-434E-8FEB-58F05049E875}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A5797B0-173C-45A6-8624-6FE8D732711A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="conversion" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="18">
   <si>
     <t>Cement</t>
   </si>
@@ -58,6 +59,27 @@
   </si>
   <si>
     <t>kg/m3</t>
+  </si>
+  <si>
+    <t>material_IRI</t>
+  </si>
+  <si>
+    <t>unit</t>
+  </si>
+  <si>
+    <t>input</t>
+  </si>
+  <si>
+    <t>amout_input</t>
+  </si>
+  <si>
+    <t>input_iri</t>
+  </si>
+  <si>
+    <t>http://data.europa.eu/ehl/cpa21/235</t>
+  </si>
+  <si>
+    <t>http://data.europa.eu/ehl/cpa21/081</t>
   </si>
 </sst>
 </file>
@@ -380,7 +402,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
@@ -458,4 +480,99 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02B33AF1-59D2-4463-B491-EB3B8F474030}">
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2">
+        <v>312</v>
+      </c>
+      <c r="F2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3">
+        <v>950</v>
+      </c>
+      <c r="F3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4">
+        <v>815</v>
+      </c>
+      <c r="F4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>